<commit_message>
new design and simulations
</commit_message>
<xml_diff>
--- a/experiment_design/store/design_matrix.xlsx
+++ b/experiment_design/store/design_matrix.xlsx
@@ -173,22 +173,22 @@
         <v>4</v>
       </c>
       <c r="E2" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F2" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G2" s="1">
         <v>80</v>
       </c>
       <c r="H2" s="1">
-        <v>1000</v>
+        <v>120000</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="J2" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
@@ -200,7 +200,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="1">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -244,7 +244,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="1">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -264,19 +264,19 @@
         <v>100</v>
       </c>
       <c r="F4" s="1">
+        <v>120</v>
+      </c>
+      <c r="G4" s="1">
+        <v>120</v>
+      </c>
+      <c r="H4" s="1">
+        <v>60000</v>
+      </c>
+      <c r="I4" s="1">
+        <v>60000</v>
+      </c>
+      <c r="J4" s="1">
         <v>40</v>
-      </c>
-      <c r="G4" s="1">
-        <v>80</v>
-      </c>
-      <c r="H4" s="1">
-        <v>500</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>5</v>
       </c>
       <c r="K4" t="s">
         <v>13</v>
@@ -288,7 +288,7 @@
         <v>2</v>
       </c>
       <c r="N4" s="1">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -332,7 +332,7 @@
         <v>2</v>
       </c>
       <c r="N5" s="1">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -349,22 +349,22 @@
         <v>4</v>
       </c>
       <c r="E6" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G6" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="K6" t="s">
         <v>13</v>
@@ -376,7 +376,7 @@
         <v>3</v>
       </c>
       <c r="N6" s="1">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -420,7 +420,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="1">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
@@ -437,22 +437,22 @@
         <v>4</v>
       </c>
       <c r="E8" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
         <v>80</v>
       </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
       <c r="H8" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="J8" s="1">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="K8" t="s">
         <v>13</v>
@@ -464,7 +464,7 @@
         <v>4</v>
       </c>
       <c r="N8" s="1">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -508,7 +508,7 @@
         <v>4</v>
       </c>
       <c r="N9" s="1">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -528,16 +528,16 @@
         <v>100</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G10" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="J10" s="1">
         <v>15</v>
@@ -552,7 +552,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="1">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
@@ -596,7 +596,7 @@
         <v>5</v>
       </c>
       <c r="N11" s="1">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -613,7 +613,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="F12" s="1">
         <v>120</v>
@@ -622,7 +622,7 @@
         <v>40</v>
       </c>
       <c r="H12" s="1">
-        <v>500</v>
+        <v>120000</v>
       </c>
       <c r="I12" s="1">
         <v>0</v>
@@ -640,7 +640,7 @@
         <v>6</v>
       </c>
       <c r="N12" s="1">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13">
@@ -684,7 +684,7 @@
         <v>6</v>
       </c>
       <c r="N13" s="1">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14">
@@ -704,19 +704,19 @@
         <v>50</v>
       </c>
       <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
         <v>120</v>
       </c>
-      <c r="G14" s="1">
-        <v>80</v>
-      </c>
       <c r="H14" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I14" s="1">
-        <v>1000</v>
+        <v>120000</v>
       </c>
       <c r="J14" s="1">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="K14" t="s">
         <v>13</v>
@@ -728,7 +728,7 @@
         <v>7</v>
       </c>
       <c r="N14" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15">
@@ -772,7 +772,7 @@
         <v>7</v>
       </c>
       <c r="N15" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16">
@@ -789,22 +789,22 @@
         <v>4</v>
       </c>
       <c r="E16" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
         <v>80</v>
       </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
       <c r="H16" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I16" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J16" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K16" t="s">
         <v>13</v>
@@ -816,7 +816,7 @@
         <v>8</v>
       </c>
       <c r="N16" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17">
@@ -860,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="N17" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18">
@@ -877,22 +877,22 @@
         <v>4</v>
       </c>
       <c r="E18" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F18" s="1">
         <v>40</v>
       </c>
       <c r="G18" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>500</v>
+        <v>20000</v>
       </c>
       <c r="I18" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J18" s="1">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="K18" t="s">
         <v>13</v>
@@ -904,7 +904,7 @@
         <v>9</v>
       </c>
       <c r="N18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -948,7 +948,7 @@
         <v>9</v>
       </c>
       <c r="N19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -965,10 +965,10 @@
         <v>4</v>
       </c>
       <c r="E20" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F20" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G20" s="1">
         <v>120</v>
@@ -980,7 +980,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="1">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="K20" t="s">
         <v>13</v>
@@ -992,7 +992,7 @@
         <v>10</v>
       </c>
       <c r="N20" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
@@ -1036,7 +1036,7 @@
         <v>10</v>
       </c>
       <c r="N21" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
@@ -1056,7 +1056,7 @@
         <v>20</v>
       </c>
       <c r="F22" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G22" s="1">
         <v>40</v>
@@ -1065,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="J22" s="1">
         <v>15</v>
@@ -1080,7 +1080,7 @@
         <v>11</v>
       </c>
       <c r="N22" s="1">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
@@ -1124,7 +1124,7 @@
         <v>11</v>
       </c>
       <c r="N23" s="1">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24">
@@ -1144,16 +1144,16 @@
         <v>5</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G24" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="H24" s="1">
-        <v>1000</v>
+        <v>80000</v>
       </c>
       <c r="I24" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="J24" s="1">
         <v>40</v>
@@ -1168,7 +1168,7 @@
         <v>12</v>
       </c>
       <c r="N24" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25">
@@ -1212,7 +1212,7 @@
         <v>12</v>
       </c>
       <c r="N25" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26">
@@ -1229,22 +1229,22 @@
         <v>4</v>
       </c>
       <c r="E26" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F26" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G26" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="H26" s="1">
-        <v>1000</v>
+        <v>120000</v>
       </c>
       <c r="I26" s="1">
-        <v>1000</v>
+        <v>60000</v>
       </c>
       <c r="J26" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K26" t="s">
         <v>13</v>
@@ -1256,7 +1256,7 @@
         <v>13</v>
       </c>
       <c r="N26" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27">
@@ -1300,7 +1300,7 @@
         <v>13</v>
       </c>
       <c r="N27" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28">
@@ -1317,7 +1317,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F28" s="1">
         <v>40</v>
@@ -1326,13 +1326,13 @@
         <v>40</v>
       </c>
       <c r="H28" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I28" s="1">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="J28" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K28" t="s">
         <v>13</v>
@@ -1344,7 +1344,7 @@
         <v>14</v>
       </c>
       <c r="N28" s="1">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29">
@@ -1388,7 +1388,7 @@
         <v>14</v>
       </c>
       <c r="N29" s="1">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30">
@@ -1405,22 +1405,22 @@
         <v>4</v>
       </c>
       <c r="E30" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F30" s="1">
         <v>80</v>
       </c>
       <c r="G30" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H30" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="I30" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J30" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K30" t="s">
         <v>13</v>
@@ -1432,7 +1432,7 @@
         <v>15</v>
       </c>
       <c r="N30" s="1">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31">
@@ -1476,7 +1476,7 @@
         <v>15</v>
       </c>
       <c r="N31" s="1">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32">
@@ -1493,7 +1493,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F32" s="1">
         <v>120</v>
@@ -1502,10 +1502,10 @@
         <v>40</v>
       </c>
       <c r="H32" s="1">
-        <v>500</v>
+        <v>120000</v>
       </c>
       <c r="I32" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J32" s="1">
         <v>40</v>
@@ -1520,7 +1520,7 @@
         <v>16</v>
       </c>
       <c r="N32" s="1">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33">
@@ -1564,7 +1564,7 @@
         <v>16</v>
       </c>
       <c r="N33" s="1">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34">
@@ -1584,19 +1584,19 @@
         <v>50</v>
       </c>
       <c r="F34" s="1">
+        <v>40</v>
+      </c>
+      <c r="G34" s="1">
         <v>80</v>
       </c>
-      <c r="G34" s="1">
-        <v>0</v>
-      </c>
       <c r="H34" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I34" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J34" s="1">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="K34" t="s">
         <v>13</v>
@@ -1608,7 +1608,7 @@
         <v>17</v>
       </c>
       <c r="N34" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
@@ -1652,7 +1652,7 @@
         <v>17</v>
       </c>
       <c r="N35" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -1669,19 +1669,19 @@
         <v>4</v>
       </c>
       <c r="E36" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F36" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G36" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="H36" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I36" s="1">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="J36" s="1">
         <v>5</v>
@@ -1696,7 +1696,7 @@
         <v>18</v>
       </c>
       <c r="N36" s="1">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -1740,7 +1740,7 @@
         <v>18</v>
       </c>
       <c r="N37" s="1">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
@@ -1760,16 +1760,16 @@
         <v>100</v>
       </c>
       <c r="F38" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G38" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H38" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I38" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J38" s="1">
         <v>40</v>
@@ -1784,7 +1784,7 @@
         <v>19</v>
       </c>
       <c r="N38" s="1">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
@@ -1828,7 +1828,7 @@
         <v>19</v>
       </c>
       <c r="N39" s="1">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40">
@@ -1851,16 +1851,16 @@
         <v>120</v>
       </c>
       <c r="G40" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H40" s="1">
-        <v>1000</v>
+        <v>60000</v>
       </c>
       <c r="I40" s="1">
         <v>0</v>
       </c>
       <c r="J40" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K40" t="s">
         <v>13</v>
@@ -1872,7 +1872,7 @@
         <v>20</v>
       </c>
       <c r="N40" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41">
@@ -1916,7 +1916,7 @@
         <v>20</v>
       </c>
       <c r="N41" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42">
@@ -1933,19 +1933,19 @@
         <v>4</v>
       </c>
       <c r="E42" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F42" s="1">
         <v>40</v>
       </c>
       <c r="G42" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H42" s="1">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="I42" s="1">
-        <v>500</v>
+        <v>40000</v>
       </c>
       <c r="J42" s="1">
         <v>5</v>
@@ -1960,7 +1960,7 @@
         <v>21</v>
       </c>
       <c r="N42" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43">
@@ -2004,7 +2004,7 @@
         <v>21</v>
       </c>
       <c r="N43" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44">
@@ -2021,22 +2021,22 @@
         <v>4</v>
       </c>
       <c r="E44" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F44" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G44" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H44" s="1">
         <v>0</v>
       </c>
       <c r="I44" s="1">
-        <v>500</v>
+        <v>20000</v>
       </c>
       <c r="J44" s="1">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="K44" t="s">
         <v>13</v>
@@ -2048,7 +2048,7 @@
         <v>22</v>
       </c>
       <c r="N44" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45">
@@ -2092,7 +2092,7 @@
         <v>22</v>
       </c>
       <c r="N45" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46">
@@ -2109,19 +2109,19 @@
         <v>4</v>
       </c>
       <c r="E46" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F46" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G46" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H46" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I46" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J46" s="1">
         <v>5</v>
@@ -2136,7 +2136,7 @@
         <v>23</v>
       </c>
       <c r="N46" s="1">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47">
@@ -2180,7 +2180,7 @@
         <v>23</v>
       </c>
       <c r="N47" s="1">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48">
@@ -2200,19 +2200,19 @@
         <v>5</v>
       </c>
       <c r="F48" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G48" s="1">
         <v>120</v>
       </c>
       <c r="H48" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I48" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J48" s="1">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="K48" t="s">
         <v>13</v>
@@ -2224,7 +2224,7 @@
         <v>24</v>
       </c>
       <c r="N48" s="1">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49">
@@ -2268,7 +2268,7 @@
         <v>24</v>
       </c>
       <c r="N49" s="1">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50">
@@ -2294,13 +2294,13 @@
         <v>80</v>
       </c>
       <c r="H50" s="1">
-        <v>500</v>
+        <v>40000</v>
       </c>
       <c r="I50" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="J50" s="1">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="K50" t="s">
         <v>13</v>
@@ -2312,7 +2312,7 @@
         <v>25</v>
       </c>
       <c r="N50" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51">
@@ -2356,7 +2356,7 @@
         <v>25</v>
       </c>
       <c r="N51" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52">
@@ -2373,19 +2373,19 @@
         <v>4</v>
       </c>
       <c r="E52" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F52" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G52" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="H52" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I52" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J52" s="1">
         <v>15</v>
@@ -2400,7 +2400,7 @@
         <v>26</v>
       </c>
       <c r="N52" s="1">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53">
@@ -2444,7 +2444,7 @@
         <v>26</v>
       </c>
       <c r="N53" s="1">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54">
@@ -2464,19 +2464,19 @@
         <v>5</v>
       </c>
       <c r="F54" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G54" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="H54" s="1">
         <v>0</v>
       </c>
       <c r="I54" s="1">
-        <v>1000</v>
+        <v>120000</v>
       </c>
       <c r="J54" s="1">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="K54" t="s">
         <v>13</v>
@@ -2488,7 +2488,7 @@
         <v>27</v>
       </c>
       <c r="N54" s="1">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55">
@@ -2532,7 +2532,7 @@
         <v>27</v>
       </c>
       <c r="N55" s="1">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56">
@@ -2552,16 +2552,16 @@
         <v>20</v>
       </c>
       <c r="F56" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G56" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H56" s="1">
         <v>0</v>
       </c>
       <c r="I56" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="J56" s="1">
         <v>5</v>
@@ -2576,7 +2576,7 @@
         <v>28</v>
       </c>
       <c r="N56" s="1">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57">
@@ -2620,7 +2620,7 @@
         <v>28</v>
       </c>
       <c r="N57" s="1">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58">
@@ -2637,19 +2637,19 @@
         <v>4</v>
       </c>
       <c r="E58" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F58" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G58" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H58" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I58" s="1">
-        <v>500</v>
+        <v>120000</v>
       </c>
       <c r="J58" s="1">
         <v>5</v>
@@ -2664,7 +2664,7 @@
         <v>29</v>
       </c>
       <c r="N58" s="1">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59">
@@ -2708,7 +2708,7 @@
         <v>29</v>
       </c>
       <c r="N59" s="1">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60">
@@ -2728,19 +2728,19 @@
         <v>100</v>
       </c>
       <c r="F60" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G60" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H60" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="I60" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="J60" s="1">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="K60" t="s">
         <v>13</v>
@@ -2752,7 +2752,7 @@
         <v>30</v>
       </c>
       <c r="N60" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61">
@@ -2796,7 +2796,7 @@
         <v>30</v>
       </c>
       <c r="N61" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62">
@@ -2813,22 +2813,22 @@
         <v>4</v>
       </c>
       <c r="E62" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F62" s="1">
         <v>120</v>
       </c>
       <c r="G62" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H62" s="1">
-        <v>1000</v>
+        <v>60000</v>
       </c>
       <c r="I62" s="1">
-        <v>500</v>
+        <v>60000</v>
       </c>
       <c r="J62" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K62" t="s">
         <v>13</v>
@@ -2840,7 +2840,7 @@
         <v>31</v>
       </c>
       <c r="N62" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63">
@@ -2884,7 +2884,7 @@
         <v>31</v>
       </c>
       <c r="N63" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64">
@@ -2901,19 +2901,19 @@
         <v>4</v>
       </c>
       <c r="E64" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F64" s="1">
         <v>80</v>
       </c>
       <c r="G64" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H64" s="1">
-        <v>1000</v>
+        <v>80000</v>
       </c>
       <c r="I64" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J64" s="1">
         <v>40</v>
@@ -2928,7 +2928,7 @@
         <v>32</v>
       </c>
       <c r="N64" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65">
@@ -2972,7 +2972,7 @@
         <v>32</v>
       </c>
       <c r="N65" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66">
@@ -2989,22 +2989,22 @@
         <v>4</v>
       </c>
       <c r="E66" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F66" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G66" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H66" s="1">
-        <v>1000</v>
+        <v>80000</v>
       </c>
       <c r="I66" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J66" s="1">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="K66" t="s">
         <v>13</v>
@@ -3077,22 +3077,22 @@
         <v>4</v>
       </c>
       <c r="E68" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F68" s="1">
+        <v>80</v>
+      </c>
+      <c r="G68" s="1">
+        <v>120</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0</v>
+      </c>
+      <c r="I68" s="1">
+        <v>120000</v>
+      </c>
+      <c r="J68" s="1">
         <v>40</v>
-      </c>
-      <c r="G68" s="1">
-        <v>40</v>
-      </c>
-      <c r="H68" s="1">
-        <v>0</v>
-      </c>
-      <c r="I68" s="1">
-        <v>1000</v>
-      </c>
-      <c r="J68" s="1">
-        <v>15</v>
       </c>
       <c r="K68" t="s">
         <v>13</v>
@@ -3104,7 +3104,7 @@
         <v>34</v>
       </c>
       <c r="N68" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69">
@@ -3148,7 +3148,7 @@
         <v>34</v>
       </c>
       <c r="N69" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70">
@@ -3165,22 +3165,22 @@
         <v>4</v>
       </c>
       <c r="E70" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F70" s="1">
+        <v>40</v>
+      </c>
+      <c r="G70" s="1">
         <v>120</v>
       </c>
-      <c r="G70" s="1">
-        <v>40</v>
-      </c>
       <c r="H70" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I70" s="1">
-        <v>500</v>
+        <v>120000</v>
       </c>
       <c r="J70" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K70" t="s">
         <v>13</v>
@@ -3192,7 +3192,7 @@
         <v>35</v>
       </c>
       <c r="N70" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71">
@@ -3236,7 +3236,7 @@
         <v>35</v>
       </c>
       <c r="N71" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72">
@@ -3253,19 +3253,19 @@
         <v>4</v>
       </c>
       <c r="E72" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F72" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G72" s="1">
         <v>40</v>
       </c>
       <c r="H72" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I72" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="J72" s="1">
         <v>40</v>
@@ -3280,7 +3280,7 @@
         <v>36</v>
       </c>
       <c r="N72" s="1">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73">
@@ -3324,7 +3324,7 @@
         <v>36</v>
       </c>
       <c r="N73" s="1">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74">
@@ -3341,22 +3341,22 @@
         <v>4</v>
       </c>
       <c r="E74" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F74" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G74" s="1">
         <v>120</v>
       </c>
       <c r="H74" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I74" s="1">
-        <v>500</v>
+        <v>60000</v>
       </c>
       <c r="J74" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K74" t="s">
         <v>13</v>
@@ -3368,7 +3368,7 @@
         <v>37</v>
       </c>
       <c r="N74" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75">
@@ -3412,7 +3412,7 @@
         <v>37</v>
       </c>
       <c r="N75" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76">
@@ -3429,22 +3429,22 @@
         <v>4</v>
       </c>
       <c r="E76" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F76" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G76" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H76" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I76" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J76" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K76" t="s">
         <v>13</v>
@@ -3456,7 +3456,7 @@
         <v>38</v>
       </c>
       <c r="N76" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77">
@@ -3500,7 +3500,7 @@
         <v>38</v>
       </c>
       <c r="N77" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78">
@@ -3520,19 +3520,19 @@
         <v>50</v>
       </c>
       <c r="F78" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G78" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H78" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I78" s="1">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="J78" s="1">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="K78" t="s">
         <v>13</v>
@@ -3544,7 +3544,7 @@
         <v>39</v>
       </c>
       <c r="N78" s="1">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79">
@@ -3588,7 +3588,7 @@
         <v>39</v>
       </c>
       <c r="N79" s="1">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80">
@@ -3605,19 +3605,19 @@
         <v>4</v>
       </c>
       <c r="E80" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F80" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G80" s="1">
         <v>80</v>
       </c>
       <c r="H80" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I80" s="1">
-        <v>500</v>
+        <v>80000</v>
       </c>
       <c r="J80" s="1">
         <v>40</v>
@@ -3632,7 +3632,7 @@
         <v>40</v>
       </c>
       <c r="N80" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81">
@@ -3676,7 +3676,7 @@
         <v>40</v>
       </c>
       <c r="N81" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82">
@@ -3693,22 +3693,22 @@
         <v>4</v>
       </c>
       <c r="E82" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F82" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G82" s="1">
         <v>80</v>
       </c>
       <c r="H82" s="1">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="I82" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J82" s="1">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="K82" t="s">
         <v>13</v>
@@ -3720,7 +3720,7 @@
         <v>41</v>
       </c>
       <c r="N82" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83">
@@ -3764,7 +3764,7 @@
         <v>41</v>
       </c>
       <c r="N83" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84">
@@ -3784,19 +3784,19 @@
         <v>100</v>
       </c>
       <c r="F84" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G84" s="1">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="H84" s="1">
-        <v>1000</v>
+        <v>60000</v>
       </c>
       <c r="I84" s="1">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="J84" s="1">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="K84" t="s">
         <v>13</v>
@@ -3808,7 +3808,7 @@
         <v>42</v>
       </c>
       <c r="N84" s="1">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="85">
@@ -3852,7 +3852,7 @@
         <v>42</v>
       </c>
       <c r="N85" s="1">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86">
@@ -3878,13 +3878,13 @@
         <v>0</v>
       </c>
       <c r="H86" s="1">
-        <v>500</v>
+        <v>40000</v>
       </c>
       <c r="I86" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J86" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K86" t="s">
         <v>13</v>
@@ -3896,7 +3896,7 @@
         <v>43</v>
       </c>
       <c r="N86" s="1">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="87">
@@ -3940,7 +3940,7 @@
         <v>43</v>
       </c>
       <c r="N87" s="1">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="88">
@@ -3960,10 +3960,10 @@
         <v>5</v>
       </c>
       <c r="F88" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G88" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="H88" s="1">
         <v>0</v>
@@ -3972,7 +3972,7 @@
         <v>0</v>
       </c>
       <c r="J88" s="1">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="K88" t="s">
         <v>13</v>
@@ -3984,7 +3984,7 @@
         <v>44</v>
       </c>
       <c r="N88" s="1">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89">
@@ -4028,7 +4028,7 @@
         <v>44</v>
       </c>
       <c r="N89" s="1">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90">
@@ -4045,22 +4045,22 @@
         <v>4</v>
       </c>
       <c r="E90" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F90" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G90" s="1">
         <v>40</v>
       </c>
       <c r="H90" s="1">
-        <v>1000</v>
+        <v>80000</v>
       </c>
       <c r="I90" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J90" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K90" t="s">
         <v>13</v>
@@ -4072,7 +4072,7 @@
         <v>45</v>
       </c>
       <c r="N90" s="1">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91">
@@ -4116,7 +4116,7 @@
         <v>45</v>
       </c>
       <c r="N91" s="1">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92">
@@ -4133,22 +4133,22 @@
         <v>4</v>
       </c>
       <c r="E92" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F92" s="1">
+        <v>80</v>
+      </c>
+      <c r="G92" s="1">
         <v>120</v>
       </c>
-      <c r="G92" s="1">
-        <v>0</v>
-      </c>
       <c r="H92" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I92" s="1">
-        <v>500</v>
+        <v>120000</v>
       </c>
       <c r="J92" s="1">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="K92" t="s">
         <v>13</v>
@@ -4160,7 +4160,7 @@
         <v>46</v>
       </c>
       <c r="N92" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93">
@@ -4204,7 +4204,7 @@
         <v>46</v>
       </c>
       <c r="N93" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="94">
@@ -4221,22 +4221,22 @@
         <v>4</v>
       </c>
       <c r="E94" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F94" s="1">
+        <v>0</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0</v>
+      </c>
+      <c r="H94" s="1">
+        <v>0</v>
+      </c>
+      <c r="I94" s="1">
+        <v>0</v>
+      </c>
+      <c r="J94" s="1">
         <v>40</v>
-      </c>
-      <c r="G94" s="1">
-        <v>120</v>
-      </c>
-      <c r="H94" s="1">
-        <v>1000</v>
-      </c>
-      <c r="I94" s="1">
-        <v>0</v>
-      </c>
-      <c r="J94" s="1">
-        <v>15</v>
       </c>
       <c r="K94" t="s">
         <v>13</v>
@@ -4248,7 +4248,7 @@
         <v>47</v>
       </c>
       <c r="N94" s="1">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="95">
@@ -4292,7 +4292,7 @@
         <v>47</v>
       </c>
       <c r="N95" s="1">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96">
@@ -4309,7 +4309,7 @@
         <v>4</v>
       </c>
       <c r="E96" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F96" s="1">
         <v>80</v>
@@ -4318,10 +4318,10 @@
         <v>80</v>
       </c>
       <c r="H96" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I96" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="J96" s="1">
         <v>15</v>
@@ -4336,7 +4336,7 @@
         <v>48</v>
       </c>
       <c r="N96" s="1">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="97">
@@ -4380,7 +4380,7 @@
         <v>48</v>
       </c>
       <c r="N97" s="1">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="98">
@@ -4397,22 +4397,22 @@
         <v>4</v>
       </c>
       <c r="E98" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F98" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G98" s="1">
         <v>80</v>
       </c>
       <c r="H98" s="1">
-        <v>1000</v>
+        <v>120000</v>
       </c>
       <c r="I98" s="1">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="J98" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="K98" t="s">
         <v>14</v>
@@ -4424,7 +4424,7 @@
         <v>1</v>
       </c>
       <c r="N98" s="1">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -4468,7 +4468,7 @@
         <v>1</v>
       </c>
       <c r="N99" s="1">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -4488,19 +4488,19 @@
         <v>100</v>
       </c>
       <c r="F100" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G100" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="H100" s="1">
-        <v>500</v>
+        <v>60000</v>
       </c>
       <c r="I100" s="1">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="J100" s="1">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="K100" t="s">
         <v>14</v>
@@ -4512,7 +4512,7 @@
         <v>2</v>
       </c>
       <c r="N100" s="1">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101">
@@ -4556,7 +4556,7 @@
         <v>2</v>
       </c>
       <c r="N101" s="1">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102">
@@ -4573,22 +4573,22 @@
         <v>4</v>
       </c>
       <c r="E102" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F102" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G102" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H102" s="1">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="I102" s="1">
         <v>0</v>
       </c>
       <c r="J102" s="1">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="K102" t="s">
         <v>14</v>
@@ -4600,7 +4600,7 @@
         <v>3</v>
       </c>
       <c r="N102" s="1">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103">
@@ -4644,7 +4644,7 @@
         <v>3</v>
       </c>
       <c r="N103" s="1">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104">
@@ -4661,22 +4661,22 @@
         <v>4</v>
       </c>
       <c r="E104" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F104" s="1">
+        <v>0</v>
+      </c>
+      <c r="G104" s="1">
         <v>80</v>
       </c>
-      <c r="G104" s="1">
-        <v>0</v>
-      </c>
       <c r="H104" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I104" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="J104" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K104" t="s">
         <v>14</v>
@@ -4688,7 +4688,7 @@
         <v>4</v>
       </c>
       <c r="N104" s="1">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105">
@@ -4732,7 +4732,7 @@
         <v>4</v>
       </c>
       <c r="N105" s="1">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106">
@@ -4752,16 +4752,16 @@
         <v>100</v>
       </c>
       <c r="F106" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G106" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="H106" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I106" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="J106" s="1">
         <v>30</v>
@@ -4776,7 +4776,7 @@
         <v>5</v>
       </c>
       <c r="N106" s="1">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="107">
@@ -4820,7 +4820,7 @@
         <v>5</v>
       </c>
       <c r="N107" s="1">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="108">
@@ -4837,7 +4837,7 @@
         <v>4</v>
       </c>
       <c r="E108" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="F108" s="1">
         <v>120</v>
@@ -4846,7 +4846,7 @@
         <v>40</v>
       </c>
       <c r="H108" s="1">
-        <v>500</v>
+        <v>120000</v>
       </c>
       <c r="I108" s="1">
         <v>0</v>
@@ -4864,7 +4864,7 @@
         <v>6</v>
       </c>
       <c r="N108" s="1">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="109">
@@ -4908,7 +4908,7 @@
         <v>6</v>
       </c>
       <c r="N109" s="1">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="110">
@@ -4928,19 +4928,19 @@
         <v>50</v>
       </c>
       <c r="F110" s="1">
+        <v>0</v>
+      </c>
+      <c r="G110" s="1">
         <v>120</v>
       </c>
-      <c r="G110" s="1">
-        <v>80</v>
-      </c>
       <c r="H110" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I110" s="1">
-        <v>1000</v>
+        <v>120000</v>
       </c>
       <c r="J110" s="1">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="K110" t="s">
         <v>14</v>
@@ -4952,7 +4952,7 @@
         <v>7</v>
       </c>
       <c r="N110" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="111">
@@ -4996,7 +4996,7 @@
         <v>7</v>
       </c>
       <c r="N111" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="112">
@@ -5013,22 +5013,22 @@
         <v>4</v>
       </c>
       <c r="E112" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="F112" s="1">
+        <v>0</v>
+      </c>
+      <c r="G112" s="1">
         <v>80</v>
       </c>
-      <c r="G112" s="1">
-        <v>0</v>
-      </c>
       <c r="H112" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I112" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J112" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K112" t="s">
         <v>14</v>
@@ -5040,7 +5040,7 @@
         <v>8</v>
       </c>
       <c r="N112" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="113">
@@ -5084,7 +5084,7 @@
         <v>8</v>
       </c>
       <c r="N113" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="114">
@@ -5101,22 +5101,22 @@
         <v>4</v>
       </c>
       <c r="E114" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F114" s="1">
         <v>40</v>
       </c>
       <c r="G114" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H114" s="1">
-        <v>500</v>
+        <v>20000</v>
       </c>
       <c r="I114" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J114" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K114" t="s">
         <v>14</v>
@@ -5128,7 +5128,7 @@
         <v>9</v>
       </c>
       <c r="N114" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115">
@@ -5172,7 +5172,7 @@
         <v>9</v>
       </c>
       <c r="N115" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
@@ -5189,10 +5189,10 @@
         <v>4</v>
       </c>
       <c r="E116" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F116" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G116" s="1">
         <v>120</v>
@@ -5204,7 +5204,7 @@
         <v>0</v>
       </c>
       <c r="J116" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K116" t="s">
         <v>14</v>
@@ -5216,7 +5216,7 @@
         <v>10</v>
       </c>
       <c r="N116" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117">
@@ -5260,7 +5260,7 @@
         <v>10</v>
       </c>
       <c r="N117" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118">
@@ -5280,7 +5280,7 @@
         <v>20</v>
       </c>
       <c r="F118" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G118" s="1">
         <v>40</v>
@@ -5289,7 +5289,7 @@
         <v>0</v>
       </c>
       <c r="I118" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="J118" s="1">
         <v>30</v>
@@ -5304,7 +5304,7 @@
         <v>11</v>
       </c>
       <c r="N118" s="1">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="119">
@@ -5348,7 +5348,7 @@
         <v>11</v>
       </c>
       <c r="N119" s="1">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="120">
@@ -5368,16 +5368,16 @@
         <v>5</v>
       </c>
       <c r="F120" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G120" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="H120" s="1">
-        <v>1000</v>
+        <v>80000</v>
       </c>
       <c r="I120" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="J120" s="1">
         <v>60</v>
@@ -5392,7 +5392,7 @@
         <v>12</v>
       </c>
       <c r="N120" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="121">
@@ -5436,7 +5436,7 @@
         <v>12</v>
       </c>
       <c r="N121" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="122">
@@ -5453,22 +5453,22 @@
         <v>4</v>
       </c>
       <c r="E122" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F122" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G122" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="H122" s="1">
-        <v>1000</v>
+        <v>120000</v>
       </c>
       <c r="I122" s="1">
-        <v>1000</v>
+        <v>60000</v>
       </c>
       <c r="J122" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="K122" t="s">
         <v>14</v>
@@ -5480,7 +5480,7 @@
         <v>13</v>
       </c>
       <c r="N122" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="123">
@@ -5524,7 +5524,7 @@
         <v>13</v>
       </c>
       <c r="N123" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="124">
@@ -5541,7 +5541,7 @@
         <v>4</v>
       </c>
       <c r="E124" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F124" s="1">
         <v>40</v>
@@ -5550,13 +5550,13 @@
         <v>40</v>
       </c>
       <c r="H124" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I124" s="1">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="J124" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K124" t="s">
         <v>14</v>
@@ -5568,7 +5568,7 @@
         <v>14</v>
       </c>
       <c r="N124" s="1">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="125">
@@ -5612,7 +5612,7 @@
         <v>14</v>
       </c>
       <c r="N125" s="1">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="126">
@@ -5629,22 +5629,22 @@
         <v>4</v>
       </c>
       <c r="E126" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F126" s="1">
         <v>80</v>
       </c>
       <c r="G126" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H126" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="I126" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J126" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="K126" t="s">
         <v>14</v>
@@ -5656,7 +5656,7 @@
         <v>15</v>
       </c>
       <c r="N126" s="1">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="127">
@@ -5700,7 +5700,7 @@
         <v>15</v>
       </c>
       <c r="N127" s="1">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="128">
@@ -5717,7 +5717,7 @@
         <v>4</v>
       </c>
       <c r="E128" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F128" s="1">
         <v>120</v>
@@ -5726,10 +5726,10 @@
         <v>40</v>
       </c>
       <c r="H128" s="1">
-        <v>500</v>
+        <v>120000</v>
       </c>
       <c r="I128" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J128" s="1">
         <v>60</v>
@@ -5744,7 +5744,7 @@
         <v>16</v>
       </c>
       <c r="N128" s="1">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="129">
@@ -5788,7 +5788,7 @@
         <v>16</v>
       </c>
       <c r="N129" s="1">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="130">
@@ -5808,19 +5808,19 @@
         <v>50</v>
       </c>
       <c r="F130" s="1">
+        <v>40</v>
+      </c>
+      <c r="G130" s="1">
         <v>80</v>
       </c>
-      <c r="G130" s="1">
-        <v>0</v>
-      </c>
       <c r="H130" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I130" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J130" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="K130" t="s">
         <v>14</v>
@@ -5832,7 +5832,7 @@
         <v>17</v>
       </c>
       <c r="N130" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131">
@@ -5876,7 +5876,7 @@
         <v>17</v>
       </c>
       <c r="N131" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132">
@@ -5893,19 +5893,19 @@
         <v>4</v>
       </c>
       <c r="E132" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F132" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G132" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="H132" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I132" s="1">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="J132" s="1">
         <v>15</v>
@@ -5920,7 +5920,7 @@
         <v>18</v>
       </c>
       <c r="N132" s="1">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133">
@@ -5964,7 +5964,7 @@
         <v>18</v>
       </c>
       <c r="N133" s="1">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134">
@@ -5984,16 +5984,16 @@
         <v>100</v>
       </c>
       <c r="F134" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G134" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H134" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I134" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J134" s="1">
         <v>60</v>
@@ -6008,7 +6008,7 @@
         <v>19</v>
       </c>
       <c r="N134" s="1">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="135">
@@ -6052,7 +6052,7 @@
         <v>19</v>
       </c>
       <c r="N135" s="1">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136">
@@ -6075,16 +6075,16 @@
         <v>120</v>
       </c>
       <c r="G136" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H136" s="1">
-        <v>1000</v>
+        <v>60000</v>
       </c>
       <c r="I136" s="1">
         <v>0</v>
       </c>
       <c r="J136" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="K136" t="s">
         <v>14</v>
@@ -6096,7 +6096,7 @@
         <v>20</v>
       </c>
       <c r="N136" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="137">
@@ -6140,7 +6140,7 @@
         <v>20</v>
       </c>
       <c r="N137" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="138">
@@ -6157,19 +6157,19 @@
         <v>4</v>
       </c>
       <c r="E138" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F138" s="1">
         <v>40</v>
       </c>
       <c r="G138" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H138" s="1">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="I138" s="1">
-        <v>500</v>
+        <v>40000</v>
       </c>
       <c r="J138" s="1">
         <v>15</v>
@@ -6184,7 +6184,7 @@
         <v>21</v>
       </c>
       <c r="N138" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="139">
@@ -6228,7 +6228,7 @@
         <v>21</v>
       </c>
       <c r="N139" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="140">
@@ -6245,22 +6245,22 @@
         <v>4</v>
       </c>
       <c r="E140" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F140" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G140" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H140" s="1">
         <v>0</v>
       </c>
       <c r="I140" s="1">
-        <v>500</v>
+        <v>20000</v>
       </c>
       <c r="J140" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="K140" t="s">
         <v>14</v>
@@ -6272,7 +6272,7 @@
         <v>22</v>
       </c>
       <c r="N140" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141">
@@ -6316,7 +6316,7 @@
         <v>22</v>
       </c>
       <c r="N141" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="142">
@@ -6333,19 +6333,19 @@
         <v>4</v>
       </c>
       <c r="E142" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F142" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G142" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H142" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I142" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J142" s="1">
         <v>15</v>
@@ -6360,7 +6360,7 @@
         <v>23</v>
       </c>
       <c r="N142" s="1">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="143">
@@ -6404,7 +6404,7 @@
         <v>23</v>
       </c>
       <c r="N143" s="1">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="144">
@@ -6424,19 +6424,19 @@
         <v>5</v>
       </c>
       <c r="F144" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G144" s="1">
         <v>120</v>
       </c>
       <c r="H144" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I144" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J144" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K144" t="s">
         <v>14</v>
@@ -6448,7 +6448,7 @@
         <v>24</v>
       </c>
       <c r="N144" s="1">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="145">
@@ -6492,7 +6492,7 @@
         <v>24</v>
       </c>
       <c r="N145" s="1">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="146">
@@ -6518,13 +6518,13 @@
         <v>80</v>
       </c>
       <c r="H146" s="1">
-        <v>500</v>
+        <v>40000</v>
       </c>
       <c r="I146" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="J146" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="K146" t="s">
         <v>14</v>
@@ -6536,7 +6536,7 @@
         <v>25</v>
       </c>
       <c r="N146" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147">
@@ -6580,7 +6580,7 @@
         <v>25</v>
       </c>
       <c r="N147" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148">
@@ -6597,19 +6597,19 @@
         <v>4</v>
       </c>
       <c r="E148" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F148" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G148" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="H148" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I148" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J148" s="1">
         <v>30</v>
@@ -6624,7 +6624,7 @@
         <v>26</v>
       </c>
       <c r="N148" s="1">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="149">
@@ -6668,7 +6668,7 @@
         <v>26</v>
       </c>
       <c r="N149" s="1">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="150">
@@ -6688,19 +6688,19 @@
         <v>5</v>
       </c>
       <c r="F150" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G150" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="H150" s="1">
         <v>0</v>
       </c>
       <c r="I150" s="1">
-        <v>1000</v>
+        <v>120000</v>
       </c>
       <c r="J150" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="K150" t="s">
         <v>14</v>
@@ -6712,7 +6712,7 @@
         <v>27</v>
       </c>
       <c r="N150" s="1">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="151">
@@ -6756,7 +6756,7 @@
         <v>27</v>
       </c>
       <c r="N151" s="1">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="152">
@@ -6776,16 +6776,16 @@
         <v>20</v>
       </c>
       <c r="F152" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G152" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H152" s="1">
         <v>0</v>
       </c>
       <c r="I152" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="J152" s="1">
         <v>15</v>
@@ -6800,7 +6800,7 @@
         <v>28</v>
       </c>
       <c r="N152" s="1">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="153">
@@ -6844,7 +6844,7 @@
         <v>28</v>
       </c>
       <c r="N153" s="1">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="154">
@@ -6861,19 +6861,19 @@
         <v>4</v>
       </c>
       <c r="E154" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F154" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G154" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H154" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I154" s="1">
-        <v>500</v>
+        <v>120000</v>
       </c>
       <c r="J154" s="1">
         <v>15</v>
@@ -6888,7 +6888,7 @@
         <v>29</v>
       </c>
       <c r="N154" s="1">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="155">
@@ -6932,7 +6932,7 @@
         <v>29</v>
       </c>
       <c r="N155" s="1">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="156">
@@ -6952,19 +6952,19 @@
         <v>100</v>
       </c>
       <c r="F156" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G156" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H156" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="I156" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="J156" s="1">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="K156" t="s">
         <v>14</v>
@@ -6976,7 +6976,7 @@
         <v>30</v>
       </c>
       <c r="N156" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="157">
@@ -7020,7 +7020,7 @@
         <v>30</v>
       </c>
       <c r="N157" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="158">
@@ -7037,22 +7037,22 @@
         <v>4</v>
       </c>
       <c r="E158" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F158" s="1">
         <v>120</v>
       </c>
       <c r="G158" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H158" s="1">
-        <v>1000</v>
+        <v>60000</v>
       </c>
       <c r="I158" s="1">
-        <v>500</v>
+        <v>60000</v>
       </c>
       <c r="J158" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K158" t="s">
         <v>14</v>
@@ -7064,7 +7064,7 @@
         <v>31</v>
       </c>
       <c r="N158" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="159">
@@ -7108,7 +7108,7 @@
         <v>31</v>
       </c>
       <c r="N159" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="160">
@@ -7125,19 +7125,19 @@
         <v>4</v>
       </c>
       <c r="E160" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F160" s="1">
         <v>80</v>
       </c>
       <c r="G160" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H160" s="1">
-        <v>1000</v>
+        <v>80000</v>
       </c>
       <c r="I160" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J160" s="1">
         <v>60</v>
@@ -7152,7 +7152,7 @@
         <v>32</v>
       </c>
       <c r="N160" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="161">
@@ -7196,7 +7196,7 @@
         <v>32</v>
       </c>
       <c r="N161" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="162">
@@ -7213,22 +7213,22 @@
         <v>4</v>
       </c>
       <c r="E162" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F162" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G162" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H162" s="1">
-        <v>1000</v>
+        <v>80000</v>
       </c>
       <c r="I162" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J162" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K162" t="s">
         <v>14</v>
@@ -7301,22 +7301,22 @@
         <v>4</v>
       </c>
       <c r="E164" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F164" s="1">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G164" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="H164" s="1">
         <v>0</v>
       </c>
       <c r="I164" s="1">
-        <v>1000</v>
+        <v>120000</v>
       </c>
       <c r="J164" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K164" t="s">
         <v>14</v>
@@ -7328,7 +7328,7 @@
         <v>34</v>
       </c>
       <c r="N164" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165">
@@ -7372,7 +7372,7 @@
         <v>34</v>
       </c>
       <c r="N165" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166">
@@ -7389,22 +7389,22 @@
         <v>4</v>
       </c>
       <c r="E166" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F166" s="1">
+        <v>40</v>
+      </c>
+      <c r="G166" s="1">
         <v>120</v>
       </c>
-      <c r="G166" s="1">
-        <v>40</v>
-      </c>
       <c r="H166" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I166" s="1">
-        <v>500</v>
+        <v>120000</v>
       </c>
       <c r="J166" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K166" t="s">
         <v>14</v>
@@ -7416,7 +7416,7 @@
         <v>35</v>
       </c>
       <c r="N166" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="167">
@@ -7460,7 +7460,7 @@
         <v>35</v>
       </c>
       <c r="N167" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="168">
@@ -7477,19 +7477,19 @@
         <v>4</v>
       </c>
       <c r="E168" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F168" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G168" s="1">
         <v>40</v>
       </c>
       <c r="H168" s="1">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I168" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="J168" s="1">
         <v>60</v>
@@ -7504,7 +7504,7 @@
         <v>36</v>
       </c>
       <c r="N168" s="1">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="169">
@@ -7548,7 +7548,7 @@
         <v>36</v>
       </c>
       <c r="N169" s="1">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="170">
@@ -7565,22 +7565,22 @@
         <v>4</v>
       </c>
       <c r="E170" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F170" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G170" s="1">
         <v>120</v>
       </c>
       <c r="H170" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I170" s="1">
-        <v>500</v>
+        <v>60000</v>
       </c>
       <c r="J170" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K170" t="s">
         <v>14</v>
@@ -7592,7 +7592,7 @@
         <v>37</v>
       </c>
       <c r="N170" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="171">
@@ -7636,7 +7636,7 @@
         <v>37</v>
       </c>
       <c r="N171" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="172">
@@ -7653,22 +7653,22 @@
         <v>4</v>
       </c>
       <c r="E172" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F172" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G172" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H172" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I172" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J172" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K172" t="s">
         <v>14</v>
@@ -7680,7 +7680,7 @@
         <v>38</v>
       </c>
       <c r="N172" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="173">
@@ -7724,7 +7724,7 @@
         <v>38</v>
       </c>
       <c r="N173" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="174">
@@ -7744,19 +7744,19 @@
         <v>50</v>
       </c>
       <c r="F174" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G174" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H174" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I174" s="1">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="J174" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K174" t="s">
         <v>14</v>
@@ -7768,7 +7768,7 @@
         <v>39</v>
       </c>
       <c r="N174" s="1">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="175">
@@ -7812,7 +7812,7 @@
         <v>39</v>
       </c>
       <c r="N175" s="1">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="176">
@@ -7829,19 +7829,19 @@
         <v>4</v>
       </c>
       <c r="E176" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F176" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G176" s="1">
         <v>80</v>
       </c>
       <c r="H176" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I176" s="1">
-        <v>500</v>
+        <v>80000</v>
       </c>
       <c r="J176" s="1">
         <v>60</v>
@@ -7856,7 +7856,7 @@
         <v>40</v>
       </c>
       <c r="N176" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="177">
@@ -7900,7 +7900,7 @@
         <v>40</v>
       </c>
       <c r="N177" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="178">
@@ -7917,22 +7917,22 @@
         <v>4</v>
       </c>
       <c r="E178" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F178" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G178" s="1">
         <v>80</v>
       </c>
       <c r="H178" s="1">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="I178" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J178" s="1">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="K178" t="s">
         <v>14</v>
@@ -7944,7 +7944,7 @@
         <v>41</v>
       </c>
       <c r="N178" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="179">
@@ -7988,7 +7988,7 @@
         <v>41</v>
       </c>
       <c r="N179" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="180">
@@ -8008,19 +8008,19 @@
         <v>100</v>
       </c>
       <c r="F180" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G180" s="1">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="H180" s="1">
-        <v>1000</v>
+        <v>60000</v>
       </c>
       <c r="I180" s="1">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="J180" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K180" t="s">
         <v>14</v>
@@ -8032,7 +8032,7 @@
         <v>42</v>
       </c>
       <c r="N180" s="1">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="181">
@@ -8076,7 +8076,7 @@
         <v>42</v>
       </c>
       <c r="N181" s="1">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="182">
@@ -8102,13 +8102,13 @@
         <v>0</v>
       </c>
       <c r="H182" s="1">
-        <v>500</v>
+        <v>40000</v>
       </c>
       <c r="I182" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J182" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="K182" t="s">
         <v>14</v>
@@ -8120,7 +8120,7 @@
         <v>43</v>
       </c>
       <c r="N182" s="1">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="183">
@@ -8164,7 +8164,7 @@
         <v>43</v>
       </c>
       <c r="N183" s="1">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="184">
@@ -8184,10 +8184,10 @@
         <v>5</v>
       </c>
       <c r="F184" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G184" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="H184" s="1">
         <v>0</v>
@@ -8196,7 +8196,7 @@
         <v>0</v>
       </c>
       <c r="J184" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="K184" t="s">
         <v>14</v>
@@ -8208,7 +8208,7 @@
         <v>44</v>
       </c>
       <c r="N184" s="1">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="185">
@@ -8252,7 +8252,7 @@
         <v>44</v>
       </c>
       <c r="N185" s="1">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="186">
@@ -8269,22 +8269,22 @@
         <v>4</v>
       </c>
       <c r="E186" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F186" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G186" s="1">
         <v>40</v>
       </c>
       <c r="H186" s="1">
-        <v>1000</v>
+        <v>80000</v>
       </c>
       <c r="I186" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J186" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="K186" t="s">
         <v>14</v>
@@ -8296,7 +8296,7 @@
         <v>45</v>
       </c>
       <c r="N186" s="1">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="187">
@@ -8340,7 +8340,7 @@
         <v>45</v>
       </c>
       <c r="N187" s="1">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="188">
@@ -8357,22 +8357,22 @@
         <v>4</v>
       </c>
       <c r="E188" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F188" s="1">
+        <v>80</v>
+      </c>
+      <c r="G188" s="1">
         <v>120</v>
       </c>
-      <c r="G188" s="1">
-        <v>0</v>
-      </c>
       <c r="H188" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I188" s="1">
-        <v>500</v>
+        <v>120000</v>
       </c>
       <c r="J188" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K188" t="s">
         <v>14</v>
@@ -8384,7 +8384,7 @@
         <v>46</v>
       </c>
       <c r="N188" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="189">
@@ -8428,7 +8428,7 @@
         <v>46</v>
       </c>
       <c r="N189" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="190">
@@ -8445,22 +8445,22 @@
         <v>4</v>
       </c>
       <c r="E190" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F190" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G190" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H190" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="I190" s="1">
         <v>0</v>
       </c>
       <c r="J190" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K190" t="s">
         <v>14</v>
@@ -8472,7 +8472,7 @@
         <v>47</v>
       </c>
       <c r="N190" s="1">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="191">
@@ -8516,7 +8516,7 @@
         <v>47</v>
       </c>
       <c r="N191" s="1">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="192">
@@ -8533,7 +8533,7 @@
         <v>4</v>
       </c>
       <c r="E192" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F192" s="1">
         <v>80</v>
@@ -8542,10 +8542,10 @@
         <v>80</v>
       </c>
       <c r="H192" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I192" s="1">
-        <v>1000</v>
+        <v>40000</v>
       </c>
       <c r="J192" s="1">
         <v>30</v>
@@ -8560,7 +8560,7 @@
         <v>48</v>
       </c>
       <c r="N192" s="1">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="193">
@@ -8604,7 +8604,7 @@
         <v>48</v>
       </c>
       <c r="N193" s="1">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
near and far treatment, update cards
</commit_message>
<xml_diff>
--- a/experiment_design/store/design_matrix.xlsx
+++ b/experiment_design/store/design_matrix.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="221">
   <si>
     <t>block</t>
   </si>
@@ -405,244 +405,256 @@
     <t>access</t>
   </si>
   <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
   </si>
   <si>
     <t>Picnic Tables</t>
   </si>
   <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Walking Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Walking Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Walking Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
   </si>
   <si>
     <t>Picnic Tables</t>
   </si>
   <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
   </si>
   <si>
     <t>Picnic Tables</t>
   </si>
   <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
   </si>
   <si>
     <t>Picnic Tables</t>
   </si>
   <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Walking Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
   </si>
   <si>
     <t>Picnic Tables</t>
   </si>
   <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Walking Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Walking Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Walking Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
   </si>
   <si>
     <t>Picnic Tables</t>
   </si>
   <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
   </si>
   <si>
     <t>Picnic Tables</t>
   </si>
   <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Tables and Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
   </si>
   <si>
     <t>Picnic Tables</t>
   </si>
   <si>
-    <t>No Access</t>
-  </si>
-  <si>
-    <t>Walking Trails</t>
-  </si>
-  <si>
-    <t>No Access</t>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Picnic Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Picnic Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Maintained Trails</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Picnic Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Trails and Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
+  </si>
+  <si>
+    <t>Picnic Tables</t>
+  </si>
+  <si>
+    <t>No Recreation</t>
   </si>
   <si>
     <t>distance</t>
@@ -651,10 +663,10 @@
     <t>treatment</t>
   </si>
   <si>
-    <t>miles</t>
-  </si>
-  <si>
-    <t>minutes</t>
+    <t>near</t>
+  </si>
+  <si>
+    <t>far</t>
   </si>
   <si>
     <t>alt_id</t>
@@ -744,19 +756,19 @@
         <v>129</v>
       </c>
       <c r="K1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="L1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="M1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="N1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="O1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2">
@@ -773,28 +785,28 @@
         <v>4</v>
       </c>
       <c r="E2" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
         <v>130</v>
       </c>
       <c r="K2" s="1">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M2" s="1">
         <v>1</v>
@@ -803,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="O2" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -841,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M3" s="1">
         <v>2</v>
@@ -850,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="O3" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -867,28 +879,28 @@
         <v>6</v>
       </c>
       <c r="E4" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F4" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="H4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K4" s="1">
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M4" s="1">
         <v>3</v>
@@ -897,7 +909,7 @@
         <v>2</v>
       </c>
       <c r="O4" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -929,13 +941,13 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M5" s="1">
         <v>4</v>
@@ -944,7 +956,7 @@
         <v>2</v>
       </c>
       <c r="O5" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -961,28 +973,28 @@
         <v>8</v>
       </c>
       <c r="E6" s="1">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="F6" s="1">
         <v>40</v>
       </c>
       <c r="G6" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K6" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="L6" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M6" s="1">
         <v>5</v>
@@ -991,7 +1003,7 @@
         <v>3</v>
       </c>
       <c r="O6" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -1023,13 +1035,13 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M7" s="1">
         <v>6</v>
@@ -1038,7 +1050,7 @@
         <v>3</v>
       </c>
       <c r="O7" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -1055,28 +1067,28 @@
         <v>10</v>
       </c>
       <c r="E8" s="1">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F8" s="1">
         <v>120</v>
       </c>
       <c r="G8" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="H8" s="1">
         <v>2</v>
       </c>
       <c r="I8" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="K8" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L8" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M8" s="1">
         <v>7</v>
@@ -1085,7 +1097,7 @@
         <v>4</v>
       </c>
       <c r="O8" s="1">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
@@ -1117,13 +1129,13 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K9" s="1">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M9" s="1">
         <v>8</v>
@@ -1132,7 +1144,7 @@
         <v>4</v>
       </c>
       <c r="O9" s="1">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
@@ -1152,25 +1164,25 @@
         <v>50</v>
       </c>
       <c r="F10" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G10" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K10" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="L10" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M10" s="1">
         <v>9</v>
@@ -1179,7 +1191,7 @@
         <v>5</v>
       </c>
       <c r="O10" s="1">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
@@ -1211,13 +1223,13 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M11" s="1">
         <v>10</v>
@@ -1226,7 +1238,7 @@
         <v>5</v>
       </c>
       <c r="O11" s="1">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12">
@@ -1246,7 +1258,7 @@
         <v>100</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G12" s="1">
         <v>40</v>
@@ -1255,16 +1267,16 @@
         <v>0</v>
       </c>
       <c r="I12" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J12" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K12" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M12" s="1">
         <v>11</v>
@@ -1305,13 +1317,13 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="K13" s="1">
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M13" s="1">
         <v>12</v>
@@ -1337,28 +1349,28 @@
         <v>16</v>
       </c>
       <c r="E14" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F14" s="1">
         <v>120</v>
       </c>
       <c r="G14" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I14" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K14" s="1">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="L14" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M14" s="1">
         <v>13</v>
@@ -1367,7 +1379,7 @@
         <v>7</v>
       </c>
       <c r="O14" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -1399,13 +1411,13 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K15" s="1">
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M15" s="1">
         <v>14</v>
@@ -1414,7 +1426,7 @@
         <v>7</v>
       </c>
       <c r="O15" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
@@ -1431,28 +1443,28 @@
         <v>18</v>
       </c>
       <c r="E16" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G16" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I16" s="1">
         <v>12</v>
       </c>
       <c r="J16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="K16" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="L16" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M16" s="1">
         <v>15</v>
@@ -1461,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="O16" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
@@ -1493,13 +1505,13 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K17" s="1">
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M17" s="1">
         <v>16</v>
@@ -1508,7 +1520,7 @@
         <v>8</v>
       </c>
       <c r="O17" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -1525,28 +1537,28 @@
         <v>20</v>
       </c>
       <c r="E18" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="F18" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G18" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="H18" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I18" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K18" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L18" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M18" s="1">
         <v>17</v>
@@ -1555,7 +1567,7 @@
         <v>9</v>
       </c>
       <c r="O18" s="1">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -1587,13 +1599,13 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K19" s="1">
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M19" s="1">
         <v>18</v>
@@ -1602,7 +1614,7 @@
         <v>9</v>
       </c>
       <c r="O19" s="1">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -1619,7 +1631,7 @@
         <v>22</v>
       </c>
       <c r="E20" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F20" s="1">
         <v>120</v>
@@ -1631,16 +1643,16 @@
         <v>12</v>
       </c>
       <c r="I20" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K20" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="L20" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M20" s="1">
         <v>19</v>
@@ -1649,7 +1661,7 @@
         <v>10</v>
       </c>
       <c r="O20" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21">
@@ -1681,13 +1693,13 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K21" s="1">
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M21" s="1">
         <v>20</v>
@@ -1696,7 +1708,7 @@
         <v>10</v>
       </c>
       <c r="O21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22">
@@ -1713,28 +1725,28 @@
         <v>24</v>
       </c>
       <c r="E22" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F22" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G22" s="1">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="H22" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K22" s="1">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="L22" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M22" s="1">
         <v>21</v>
@@ -1743,7 +1755,7 @@
         <v>11</v>
       </c>
       <c r="O22" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23">
@@ -1781,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M23" s="1">
         <v>22</v>
@@ -1790,7 +1802,7 @@
         <v>11</v>
       </c>
       <c r="O23" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24">
@@ -1807,28 +1819,28 @@
         <v>26</v>
       </c>
       <c r="E24" s="1">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G24" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
       </c>
       <c r="I24" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K24" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="L24" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M24" s="1">
         <v>23</v>
@@ -1837,7 +1849,7 @@
         <v>12</v>
       </c>
       <c r="O24" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25">
@@ -1869,13 +1881,13 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K25" s="1">
         <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M25" s="1">
         <v>24</v>
@@ -1884,7 +1896,7 @@
         <v>12</v>
       </c>
       <c r="O25" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26">
@@ -1901,28 +1913,28 @@
         <v>28</v>
       </c>
       <c r="E26" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F26" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G26" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="H26" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I26" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K26" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="L26" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M26" s="1">
         <v>25</v>
@@ -1931,7 +1943,7 @@
         <v>13</v>
       </c>
       <c r="O26" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
@@ -1963,13 +1975,13 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K27" s="1">
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M27" s="1">
         <v>26</v>
@@ -1978,7 +1990,7 @@
         <v>13</v>
       </c>
       <c r="O27" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
@@ -1995,28 +2007,28 @@
         <v>30</v>
       </c>
       <c r="E28" s="1">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F28" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G28" s="1">
         <v>40</v>
       </c>
       <c r="H28" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I28" s="1">
         <v>12</v>
       </c>
       <c r="J28" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K28" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="L28" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M28" s="1">
         <v>27</v>
@@ -2025,7 +2037,7 @@
         <v>14</v>
       </c>
       <c r="O28" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29">
@@ -2057,13 +2069,13 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K29" s="1">
         <v>0</v>
       </c>
       <c r="L29" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M29" s="1">
         <v>28</v>
@@ -2072,7 +2084,7 @@
         <v>14</v>
       </c>
       <c r="O29" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
@@ -2089,28 +2101,28 @@
         <v>32</v>
       </c>
       <c r="E30" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F30" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G30" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="H30" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I30" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K30" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L30" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M30" s="1">
         <v>29</v>
@@ -2119,7 +2131,7 @@
         <v>15</v>
       </c>
       <c r="O30" s="1">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
@@ -2151,13 +2163,13 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K31" s="1">
         <v>0</v>
       </c>
       <c r="L31" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M31" s="1">
         <v>30</v>
@@ -2166,7 +2178,7 @@
         <v>15</v>
       </c>
       <c r="O31" s="1">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32">
@@ -2183,28 +2195,28 @@
         <v>34</v>
       </c>
       <c r="E32" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F32" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G32" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H32" s="1">
+        <v>2</v>
+      </c>
+      <c r="I32" s="1">
         <v>6</v>
       </c>
-      <c r="I32" s="1">
-        <v>0</v>
-      </c>
       <c r="J32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K32" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="L32" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M32" s="1">
         <v>31</v>
@@ -2213,7 +2225,7 @@
         <v>16</v>
       </c>
       <c r="O32" s="1">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33">
@@ -2251,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="L33" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M33" s="1">
         <v>32</v>
@@ -2260,7 +2272,7 @@
         <v>16</v>
       </c>
       <c r="O33" s="1">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34">
@@ -2277,19 +2289,19 @@
         <v>36</v>
       </c>
       <c r="E34" s="1">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="F34" s="1">
         <v>40</v>
       </c>
       <c r="G34" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H34" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I34" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J34" t="s">
         <v>151</v>
@@ -2298,7 +2310,7 @@
         <v>10</v>
       </c>
       <c r="L34" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M34" s="1">
         <v>33</v>
@@ -2307,7 +2319,7 @@
         <v>17</v>
       </c>
       <c r="O34" s="1">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35">
@@ -2345,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="L35" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M35" s="1">
         <v>34</v>
@@ -2354,7 +2366,7 @@
         <v>17</v>
       </c>
       <c r="O35" s="1">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36">
@@ -2371,28 +2383,28 @@
         <v>38</v>
       </c>
       <c r="E36" s="1">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="F36" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G36" s="1">
         <v>40</v>
       </c>
       <c r="H36" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I36" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J36" t="s">
         <v>152</v>
       </c>
       <c r="K36" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L36" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M36" s="1">
         <v>35</v>
@@ -2401,7 +2413,7 @@
         <v>18</v>
       </c>
       <c r="O36" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37">
@@ -2439,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="L37" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M37" s="1">
         <v>36</v>
@@ -2448,7 +2460,7 @@
         <v>18</v>
       </c>
       <c r="O37" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38">
@@ -2465,28 +2477,28 @@
         <v>40</v>
       </c>
       <c r="E38" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="F38" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G38" s="1">
         <v>80</v>
       </c>
       <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
         <v>12</v>
       </c>
-      <c r="I38" s="1">
-        <v>0</v>
-      </c>
       <c r="J38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K38" s="1">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="L38" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M38" s="1">
         <v>37</v>
@@ -2527,13 +2539,13 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K39" s="1">
         <v>0</v>
       </c>
       <c r="L39" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M39" s="1">
         <v>38</v>
@@ -2559,28 +2571,28 @@
         <v>42</v>
       </c>
       <c r="E40" s="1">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="F40" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G40" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H40" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I40" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K40" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="L40" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M40" s="1">
         <v>39</v>
@@ -2589,7 +2601,7 @@
         <v>20</v>
       </c>
       <c r="O40" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -2627,7 +2639,7 @@
         <v>0</v>
       </c>
       <c r="L41" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M41" s="1">
         <v>40</v>
@@ -2636,7 +2648,7 @@
         <v>20</v>
       </c>
       <c r="O41" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
@@ -2653,28 +2665,28 @@
         <v>44</v>
       </c>
       <c r="E42" s="1">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="F42" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G42" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H42" s="1">
         <v>12</v>
       </c>
       <c r="I42" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="K42" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="L42" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M42" s="1">
         <v>41</v>
@@ -2683,7 +2695,7 @@
         <v>21</v>
       </c>
       <c r="O42" s="1">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -2715,13 +2727,13 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K43" s="1">
         <v>0</v>
       </c>
       <c r="L43" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M43" s="1">
         <v>42</v>
@@ -2730,7 +2742,7 @@
         <v>21</v>
       </c>
       <c r="O43" s="1">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
@@ -2747,28 +2759,28 @@
         <v>46</v>
       </c>
       <c r="E44" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F44" s="1">
+        <v>80</v>
+      </c>
+      <c r="G44" s="1">
         <v>120</v>
       </c>
-      <c r="G44" s="1">
-        <v>0</v>
-      </c>
       <c r="H44" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I44" s="1">
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="K44" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L44" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M44" s="1">
         <v>43</v>
@@ -2777,7 +2789,7 @@
         <v>22</v>
       </c>
       <c r="O44" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45">
@@ -2809,13 +2821,13 @@
         <v>0</v>
       </c>
       <c r="J45" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="K45" s="1">
         <v>0</v>
       </c>
       <c r="L45" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M45" s="1">
         <v>44</v>
@@ -2824,7 +2836,7 @@
         <v>22</v>
       </c>
       <c r="O45" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46">
@@ -2841,28 +2853,28 @@
         <v>48</v>
       </c>
       <c r="E46" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="F46" s="1">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G46" s="1">
         <v>120</v>
       </c>
       <c r="H46" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I46" s="1">
         <v>0</v>
       </c>
       <c r="J46" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="K46" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L46" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M46" s="1">
         <v>45</v>
@@ -2871,7 +2883,7 @@
         <v>23</v>
       </c>
       <c r="O46" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47">
@@ -2903,13 +2915,13 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="K47" s="1">
         <v>0</v>
       </c>
       <c r="L47" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M47" s="1">
         <v>46</v>
@@ -2918,7 +2930,7 @@
         <v>23</v>
       </c>
       <c r="O47" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48">
@@ -2935,10 +2947,10 @@
         <v>50</v>
       </c>
       <c r="E48" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F48" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G48" s="1">
         <v>120</v>
@@ -2947,16 +2959,16 @@
         <v>0</v>
       </c>
       <c r="I48" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J48" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="K48" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L48" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M48" s="1">
         <v>47</v>
@@ -2965,7 +2977,7 @@
         <v>24</v>
       </c>
       <c r="O48" s="1">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49">
@@ -2997,13 +3009,13 @@
         <v>0</v>
       </c>
       <c r="J49" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="K49" s="1">
         <v>0</v>
       </c>
       <c r="L49" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M49" s="1">
         <v>48</v>
@@ -3012,7 +3024,7 @@
         <v>24</v>
       </c>
       <c r="O49" s="1">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50">
@@ -3029,28 +3041,28 @@
         <v>52</v>
       </c>
       <c r="E50" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="F50" s="1">
         <v>80</v>
       </c>
       <c r="G50" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H50" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I50" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J50" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="K50" s="1">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="L50" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M50" s="1">
         <v>49</v>
@@ -3059,7 +3071,7 @@
         <v>25</v>
       </c>
       <c r="O50" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
@@ -3091,13 +3103,13 @@
         <v>0</v>
       </c>
       <c r="J51" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="K51" s="1">
         <v>0</v>
       </c>
       <c r="L51" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M51" s="1">
         <v>50</v>
@@ -3106,7 +3118,7 @@
         <v>25</v>
       </c>
       <c r="O51" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52">
@@ -3123,28 +3135,28 @@
         <v>54</v>
       </c>
       <c r="E52" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F52" s="1">
+        <v>40</v>
+      </c>
+      <c r="G52" s="1">
         <v>120</v>
       </c>
-      <c r="G52" s="1">
-        <v>0</v>
-      </c>
       <c r="H52" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I52" s="1">
         <v>0</v>
       </c>
       <c r="J52" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="K52" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L52" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M52" s="1">
         <v>51</v>
@@ -3153,7 +3165,7 @@
         <v>26</v>
       </c>
       <c r="O52" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53">
@@ -3185,13 +3197,13 @@
         <v>0</v>
       </c>
       <c r="J53" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="K53" s="1">
         <v>0</v>
       </c>
       <c r="L53" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M53" s="1">
         <v>52</v>
@@ -3200,7 +3212,7 @@
         <v>26</v>
       </c>
       <c r="O53" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
@@ -3217,28 +3229,28 @@
         <v>56</v>
       </c>
       <c r="E54" s="1">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="F54" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G54" s="1">
         <v>120</v>
       </c>
       <c r="H54" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I54" s="1">
         <v>12</v>
       </c>
       <c r="J54" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="K54" s="1">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="L54" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M54" s="1">
         <v>53</v>
@@ -3247,7 +3259,7 @@
         <v>27</v>
       </c>
       <c r="O54" s="1">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55">
@@ -3279,13 +3291,13 @@
         <v>0</v>
       </c>
       <c r="J55" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="K55" s="1">
         <v>0</v>
       </c>
       <c r="L55" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M55" s="1">
         <v>54</v>
@@ -3294,7 +3306,7 @@
         <v>27</v>
       </c>
       <c r="O55" s="1">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56">
@@ -3311,28 +3323,28 @@
         <v>58</v>
       </c>
       <c r="E56" s="1">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="F56" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G56" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="H56" s="1">
+        <v>0</v>
+      </c>
+      <c r="I56" s="1">
         <v>12</v>
       </c>
-      <c r="I56" s="1">
-        <v>6</v>
-      </c>
       <c r="J56" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="K56" s="1">
         <v>10</v>
       </c>
       <c r="L56" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M56" s="1">
         <v>55</v>
@@ -3341,7 +3353,7 @@
         <v>28</v>
       </c>
       <c r="O56" s="1">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57">
@@ -3373,13 +3385,13 @@
         <v>0</v>
       </c>
       <c r="J57" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="K57" s="1">
         <v>0</v>
       </c>
       <c r="L57" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M57" s="1">
         <v>56</v>
@@ -3388,7 +3400,7 @@
         <v>28</v>
       </c>
       <c r="O57" s="1">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58">
@@ -3405,28 +3417,28 @@
         <v>60</v>
       </c>
       <c r="E58" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F58" s="1">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G58" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H58" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I58" s="1">
         <v>0</v>
       </c>
       <c r="J58" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="K58" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="L58" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M58" s="1">
         <v>57</v>
@@ -3435,7 +3447,7 @@
         <v>29</v>
       </c>
       <c r="O58" s="1">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59">
@@ -3467,13 +3479,13 @@
         <v>0</v>
       </c>
       <c r="J59" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="K59" s="1">
         <v>0</v>
       </c>
       <c r="L59" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M59" s="1">
         <v>58</v>
@@ -3482,7 +3494,7 @@
         <v>29</v>
       </c>
       <c r="O59" s="1">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60">
@@ -3502,25 +3514,25 @@
         <v>20</v>
       </c>
       <c r="F60" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G60" s="1">
         <v>80</v>
       </c>
       <c r="H60" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I60" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J60" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K60" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="L60" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M60" s="1">
         <v>59</v>
@@ -3529,7 +3541,7 @@
         <v>30</v>
       </c>
       <c r="O60" s="1">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61">
@@ -3561,13 +3573,13 @@
         <v>0</v>
       </c>
       <c r="J61" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="K61" s="1">
         <v>0</v>
       </c>
       <c r="L61" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M61" s="1">
         <v>60</v>
@@ -3576,7 +3588,7 @@
         <v>30</v>
       </c>
       <c r="O61" s="1">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62">
@@ -3593,28 +3605,28 @@
         <v>64</v>
       </c>
       <c r="E62" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F62" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G62" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H62" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I62" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J62" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="K62" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L62" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M62" s="1">
         <v>1</v>
@@ -3623,7 +3635,7 @@
         <v>1</v>
       </c>
       <c r="O62" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63">
@@ -3655,13 +3667,13 @@
         <v>0</v>
       </c>
       <c r="J63" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="K63" s="1">
         <v>0</v>
       </c>
       <c r="L63" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M63" s="1">
         <v>2</v>
@@ -3670,7 +3682,7 @@
         <v>1</v>
       </c>
       <c r="O63" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
@@ -3687,28 +3699,28 @@
         <v>66</v>
       </c>
       <c r="E64" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F64" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G64" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="H64" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I64" s="1">
         <v>2</v>
       </c>
       <c r="J64" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K64" s="1">
         <v>15</v>
       </c>
       <c r="L64" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M64" s="1">
         <v>3</v>
@@ -3717,7 +3729,7 @@
         <v>2</v>
       </c>
       <c r="O64" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65">
@@ -3755,7 +3767,7 @@
         <v>0</v>
       </c>
       <c r="L65" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M65" s="1">
         <v>4</v>
@@ -3764,7 +3776,7 @@
         <v>2</v>
       </c>
       <c r="O65" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66">
@@ -3781,28 +3793,28 @@
         <v>68</v>
       </c>
       <c r="E66" s="1">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="F66" s="1">
         <v>40</v>
       </c>
       <c r="G66" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="H66" s="1">
         <v>0</v>
       </c>
       <c r="I66" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J66" t="s">
         <v>174</v>
       </c>
       <c r="K66" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L66" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M66" s="1">
         <v>5</v>
@@ -3811,7 +3823,7 @@
         <v>3</v>
       </c>
       <c r="O66" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67">
@@ -3849,7 +3861,7 @@
         <v>0</v>
       </c>
       <c r="L67" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M67" s="1">
         <v>6</v>
@@ -3858,7 +3870,7 @@
         <v>3</v>
       </c>
       <c r="O67" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68">
@@ -3875,28 +3887,28 @@
         <v>70</v>
       </c>
       <c r="E68" s="1">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F68" s="1">
         <v>120</v>
       </c>
       <c r="G68" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="H68" s="1">
         <v>2</v>
       </c>
       <c r="I68" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K68" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L68" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M68" s="1">
         <v>7</v>
@@ -3905,7 +3917,7 @@
         <v>4</v>
       </c>
       <c r="O68" s="1">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69">
@@ -3937,13 +3949,13 @@
         <v>0</v>
       </c>
       <c r="J69" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K69" s="1">
         <v>0</v>
       </c>
       <c r="L69" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M69" s="1">
         <v>8</v>
@@ -3952,7 +3964,7 @@
         <v>4</v>
       </c>
       <c r="O69" s="1">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70">
@@ -3972,25 +3984,25 @@
         <v>50</v>
       </c>
       <c r="F70" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G70" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="H70" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I70" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J70" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K70" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L70" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M70" s="1">
         <v>9</v>
@@ -3999,7 +4011,7 @@
         <v>5</v>
       </c>
       <c r="O70" s="1">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="71">
@@ -4031,13 +4043,13 @@
         <v>0</v>
       </c>
       <c r="J71" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K71" s="1">
         <v>0</v>
       </c>
       <c r="L71" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M71" s="1">
         <v>10</v>
@@ -4046,7 +4058,7 @@
         <v>5</v>
       </c>
       <c r="O71" s="1">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72">
@@ -4066,7 +4078,7 @@
         <v>100</v>
       </c>
       <c r="F72" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G72" s="1">
         <v>40</v>
@@ -4075,16 +4087,16 @@
         <v>0</v>
       </c>
       <c r="I72" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J72" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K72" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="L72" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M72" s="1">
         <v>11</v>
@@ -4125,13 +4137,13 @@
         <v>0</v>
       </c>
       <c r="J73" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K73" s="1">
         <v>0</v>
       </c>
       <c r="L73" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M73" s="1">
         <v>12</v>
@@ -4157,28 +4169,28 @@
         <v>76</v>
       </c>
       <c r="E74" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F74" s="1">
         <v>120</v>
       </c>
       <c r="G74" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H74" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I74" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J74" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K74" s="1">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="L74" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M74" s="1">
         <v>13</v>
@@ -4187,7 +4199,7 @@
         <v>7</v>
       </c>
       <c r="O74" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75">
@@ -4219,13 +4231,13 @@
         <v>0</v>
       </c>
       <c r="J75" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K75" s="1">
         <v>0</v>
       </c>
       <c r="L75" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M75" s="1">
         <v>14</v>
@@ -4234,7 +4246,7 @@
         <v>7</v>
       </c>
       <c r="O75" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
@@ -4251,28 +4263,28 @@
         <v>78</v>
       </c>
       <c r="E76" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F76" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G76" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H76" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I76" s="1">
         <v>12</v>
       </c>
       <c r="J76" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K76" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L76" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M76" s="1">
         <v>15</v>
@@ -4281,7 +4293,7 @@
         <v>8</v>
       </c>
       <c r="O76" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77">
@@ -4319,7 +4331,7 @@
         <v>0</v>
       </c>
       <c r="L77" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M77" s="1">
         <v>16</v>
@@ -4328,7 +4340,7 @@
         <v>8</v>
       </c>
       <c r="O77" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78">
@@ -4345,19 +4357,19 @@
         <v>80</v>
       </c>
       <c r="E78" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="F78" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G78" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="H78" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I78" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J78" t="s">
         <v>182</v>
@@ -4366,7 +4378,7 @@
         <v>30</v>
       </c>
       <c r="L78" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M78" s="1">
         <v>17</v>
@@ -4375,7 +4387,7 @@
         <v>9</v>
       </c>
       <c r="O78" s="1">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79">
@@ -4413,7 +4425,7 @@
         <v>0</v>
       </c>
       <c r="L79" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M79" s="1">
         <v>18</v>
@@ -4422,7 +4434,7 @@
         <v>9</v>
       </c>
       <c r="O79" s="1">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80">
@@ -4439,7 +4451,7 @@
         <v>82</v>
       </c>
       <c r="E80" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F80" s="1">
         <v>120</v>
@@ -4451,16 +4463,16 @@
         <v>12</v>
       </c>
       <c r="I80" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J80" t="s">
         <v>183</v>
       </c>
       <c r="K80" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="L80" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M80" s="1">
         <v>19</v>
@@ -4469,7 +4481,7 @@
         <v>10</v>
       </c>
       <c r="O80" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81">
@@ -4507,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="L81" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M81" s="1">
         <v>20</v>
@@ -4516,7 +4528,7 @@
         <v>10</v>
       </c>
       <c r="O81" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82">
@@ -4533,28 +4545,28 @@
         <v>84</v>
       </c>
       <c r="E82" s="1">
+        <v>50</v>
+      </c>
+      <c r="F82" s="1">
+        <v>40</v>
+      </c>
+      <c r="G82" s="1">
+        <v>80</v>
+      </c>
+      <c r="H82" s="1">
+        <v>0</v>
+      </c>
+      <c r="I82" s="1">
+        <v>12</v>
+      </c>
+      <c r="J82" t="s">
+        <v>184</v>
+      </c>
+      <c r="K82" s="1">
         <v>20</v>
       </c>
-      <c r="F82" s="1">
-        <v>120</v>
-      </c>
-      <c r="G82" s="1">
-        <v>40</v>
-      </c>
-      <c r="H82" s="1">
-        <v>2</v>
-      </c>
-      <c r="I82" s="1">
-        <v>0</v>
-      </c>
-      <c r="J82" t="s">
-        <v>183</v>
-      </c>
-      <c r="K82" s="1">
-        <v>60</v>
-      </c>
       <c r="L82" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M82" s="1">
         <v>21</v>
@@ -4563,7 +4575,7 @@
         <v>11</v>
       </c>
       <c r="O82" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83">
@@ -4595,13 +4607,13 @@
         <v>0</v>
       </c>
       <c r="J83" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="K83" s="1">
         <v>0</v>
       </c>
       <c r="L83" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M83" s="1">
         <v>22</v>
@@ -4610,7 +4622,7 @@
         <v>11</v>
       </c>
       <c r="O83" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84">
@@ -4627,28 +4639,28 @@
         <v>86</v>
       </c>
       <c r="E84" s="1">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="F84" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G84" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="H84" s="1">
         <v>0</v>
       </c>
       <c r="I84" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J84" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K84" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L84" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M84" s="1">
         <v>23</v>
@@ -4657,7 +4669,7 @@
         <v>12</v>
       </c>
       <c r="O84" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="85">
@@ -4695,7 +4707,7 @@
         <v>0</v>
       </c>
       <c r="L85" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M85" s="1">
         <v>24</v>
@@ -4704,7 +4716,7 @@
         <v>12</v>
       </c>
       <c r="O85" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86">
@@ -4721,28 +4733,28 @@
         <v>88</v>
       </c>
       <c r="E86" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F86" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G86" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="H86" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I86" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J86" t="s">
         <v>186</v>
       </c>
       <c r="K86" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="L86" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M86" s="1">
         <v>25</v>
@@ -4751,7 +4763,7 @@
         <v>13</v>
       </c>
       <c r="O86" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87">
@@ -4789,7 +4801,7 @@
         <v>0</v>
       </c>
       <c r="L87" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M87" s="1">
         <v>26</v>
@@ -4798,7 +4810,7 @@
         <v>13</v>
       </c>
       <c r="O87" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88">
@@ -4815,16 +4827,16 @@
         <v>90</v>
       </c>
       <c r="E88" s="1">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F88" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G88" s="1">
         <v>40</v>
       </c>
       <c r="H88" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I88" s="1">
         <v>12</v>
@@ -4833,10 +4845,10 @@
         <v>188</v>
       </c>
       <c r="K88" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="L88" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M88" s="1">
         <v>27</v>
@@ -4845,7 +4857,7 @@
         <v>14</v>
       </c>
       <c r="O88" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89">
@@ -4883,7 +4895,7 @@
         <v>0</v>
       </c>
       <c r="L89" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M89" s="1">
         <v>28</v>
@@ -4892,7 +4904,7 @@
         <v>14</v>
       </c>
       <c r="O89" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90">
@@ -4909,28 +4921,28 @@
         <v>92</v>
       </c>
       <c r="E90" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F90" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G90" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="H90" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I90" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J90" t="s">
         <v>190</v>
       </c>
       <c r="K90" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="L90" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M90" s="1">
         <v>29</v>
@@ -4939,7 +4951,7 @@
         <v>15</v>
       </c>
       <c r="O90" s="1">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91">
@@ -4977,7 +4989,7 @@
         <v>0</v>
       </c>
       <c r="L91" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M91" s="1">
         <v>30</v>
@@ -4986,7 +4998,7 @@
         <v>15</v>
       </c>
       <c r="O91" s="1">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92">
@@ -5003,28 +5015,28 @@
         <v>94</v>
       </c>
       <c r="E92" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F92" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G92" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H92" s="1">
+        <v>2</v>
+      </c>
+      <c r="I92" s="1">
         <v>6</v>
       </c>
-      <c r="I92" s="1">
-        <v>0</v>
-      </c>
       <c r="J92" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K92" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="L92" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M92" s="1">
         <v>31</v>
@@ -5033,7 +5045,7 @@
         <v>16</v>
       </c>
       <c r="O92" s="1">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="93">
@@ -5065,13 +5077,13 @@
         <v>0</v>
       </c>
       <c r="J93" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K93" s="1">
         <v>0</v>
       </c>
       <c r="L93" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M93" s="1">
         <v>32</v>
@@ -5080,7 +5092,7 @@
         <v>16</v>
       </c>
       <c r="O93" s="1">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94">
@@ -5097,28 +5109,28 @@
         <v>96</v>
       </c>
       <c r="E94" s="1">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="F94" s="1">
         <v>40</v>
       </c>
       <c r="G94" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H94" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I94" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J94" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K94" s="1">
         <v>15</v>
       </c>
       <c r="L94" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M94" s="1">
         <v>33</v>
@@ -5127,7 +5139,7 @@
         <v>17</v>
       </c>
       <c r="O94" s="1">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="95">
@@ -5159,13 +5171,13 @@
         <v>0</v>
       </c>
       <c r="J95" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="K95" s="1">
         <v>0</v>
       </c>
       <c r="L95" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M95" s="1">
         <v>34</v>
@@ -5174,7 +5186,7 @@
         <v>17</v>
       </c>
       <c r="O95" s="1">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96">
@@ -5191,28 +5203,28 @@
         <v>98</v>
       </c>
       <c r="E96" s="1">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="F96" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G96" s="1">
         <v>40</v>
       </c>
       <c r="H96" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I96" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J96" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="K96" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L96" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M96" s="1">
         <v>35</v>
@@ -5221,7 +5233,7 @@
         <v>18</v>
       </c>
       <c r="O96" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="97">
@@ -5253,13 +5265,13 @@
         <v>0</v>
       </c>
       <c r="J97" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="K97" s="1">
         <v>0</v>
       </c>
       <c r="L97" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M97" s="1">
         <v>36</v>
@@ -5268,7 +5280,7 @@
         <v>18</v>
       </c>
       <c r="O97" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98">
@@ -5285,28 +5297,28 @@
         <v>100</v>
       </c>
       <c r="E98" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="F98" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G98" s="1">
         <v>80</v>
       </c>
       <c r="H98" s="1">
+        <v>0</v>
+      </c>
+      <c r="I98" s="1">
         <v>12</v>
       </c>
-      <c r="I98" s="1">
-        <v>0</v>
-      </c>
       <c r="J98" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K98" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L98" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M98" s="1">
         <v>37</v>
@@ -5353,7 +5365,7 @@
         <v>0</v>
       </c>
       <c r="L99" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M99" s="1">
         <v>38</v>
@@ -5379,28 +5391,28 @@
         <v>102</v>
       </c>
       <c r="E100" s="1">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="F100" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G100" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H100" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I100" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J100" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K100" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L100" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M100" s="1">
         <v>39</v>
@@ -5409,7 +5421,7 @@
         <v>20</v>
       </c>
       <c r="O100" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
@@ -5441,13 +5453,13 @@
         <v>0</v>
       </c>
       <c r="J101" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="K101" s="1">
         <v>0</v>
       </c>
       <c r="L101" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M101" s="1">
         <v>40</v>
@@ -5456,7 +5468,7 @@
         <v>20</v>
       </c>
       <c r="O101" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
@@ -5473,28 +5485,28 @@
         <v>104</v>
       </c>
       <c r="E102" s="1">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="F102" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G102" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H102" s="1">
         <v>12</v>
       </c>
       <c r="I102" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J102" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="K102" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L102" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M102" s="1">
         <v>41</v>
@@ -5503,7 +5515,7 @@
         <v>21</v>
       </c>
       <c r="O102" s="1">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103">
@@ -5535,13 +5547,13 @@
         <v>0</v>
       </c>
       <c r="J103" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="K103" s="1">
         <v>0</v>
       </c>
       <c r="L103" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M103" s="1">
         <v>42</v>
@@ -5550,7 +5562,7 @@
         <v>21</v>
       </c>
       <c r="O103" s="1">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104">
@@ -5567,28 +5579,28 @@
         <v>106</v>
       </c>
       <c r="E104" s="1">
+        <v>100</v>
+      </c>
+      <c r="F104" s="1">
+        <v>80</v>
+      </c>
+      <c r="G104" s="1">
+        <v>120</v>
+      </c>
+      <c r="H104" s="1">
+        <v>6</v>
+      </c>
+      <c r="I104" s="1">
+        <v>0</v>
+      </c>
+      <c r="J104" t="s">
+        <v>200</v>
+      </c>
+      <c r="K104" s="1">
         <v>20</v>
       </c>
-      <c r="F104" s="1">
-        <v>120</v>
-      </c>
-      <c r="G104" s="1">
-        <v>0</v>
-      </c>
-      <c r="H104" s="1">
-        <v>12</v>
-      </c>
-      <c r="I104" s="1">
-        <v>0</v>
-      </c>
-      <c r="J104" t="s">
-        <v>196</v>
-      </c>
-      <c r="K104" s="1">
-        <v>15</v>
-      </c>
       <c r="L104" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M104" s="1">
         <v>43</v>
@@ -5597,7 +5609,7 @@
         <v>22</v>
       </c>
       <c r="O104" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105">
@@ -5629,13 +5641,13 @@
         <v>0</v>
       </c>
       <c r="J105" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="K105" s="1">
         <v>0</v>
       </c>
       <c r="L105" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M105" s="1">
         <v>44</v>
@@ -5644,7 +5656,7 @@
         <v>22</v>
       </c>
       <c r="O105" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106">
@@ -5661,28 +5673,28 @@
         <v>108</v>
       </c>
       <c r="E106" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="F106" s="1">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G106" s="1">
         <v>120</v>
       </c>
       <c r="H106" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I106" s="1">
         <v>0</v>
       </c>
       <c r="J106" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="K106" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="L106" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M106" s="1">
         <v>45</v>
@@ -5691,7 +5703,7 @@
         <v>23</v>
       </c>
       <c r="O106" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="107">
@@ -5723,13 +5735,13 @@
         <v>0</v>
       </c>
       <c r="J107" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="K107" s="1">
         <v>0</v>
       </c>
       <c r="L107" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M107" s="1">
         <v>46</v>
@@ -5738,7 +5750,7 @@
         <v>23</v>
       </c>
       <c r="O107" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108">
@@ -5755,10 +5767,10 @@
         <v>110</v>
       </c>
       <c r="E108" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F108" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G108" s="1">
         <v>120</v>
@@ -5767,16 +5779,16 @@
         <v>0</v>
       </c>
       <c r="I108" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J108" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="K108" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L108" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M108" s="1">
         <v>47</v>
@@ -5785,7 +5797,7 @@
         <v>24</v>
       </c>
       <c r="O108" s="1">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="109">
@@ -5817,13 +5829,13 @@
         <v>0</v>
       </c>
       <c r="J109" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="K109" s="1">
         <v>0</v>
       </c>
       <c r="L109" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M109" s="1">
         <v>48</v>
@@ -5832,7 +5844,7 @@
         <v>24</v>
       </c>
       <c r="O109" s="1">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="110">
@@ -5849,28 +5861,28 @@
         <v>112</v>
       </c>
       <c r="E110" s="1">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="F110" s="1">
         <v>80</v>
       </c>
       <c r="G110" s="1">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="H110" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I110" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J110" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="K110" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L110" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M110" s="1">
         <v>49</v>
@@ -5879,7 +5891,7 @@
         <v>25</v>
       </c>
       <c r="O110" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111">
@@ -5911,13 +5923,13 @@
         <v>0</v>
       </c>
       <c r="J111" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="K111" s="1">
         <v>0</v>
       </c>
       <c r="L111" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M111" s="1">
         <v>50</v>
@@ -5926,7 +5938,7 @@
         <v>25</v>
       </c>
       <c r="O111" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112">
@@ -5943,28 +5955,28 @@
         <v>114</v>
       </c>
       <c r="E112" s="1">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F112" s="1">
+        <v>40</v>
+      </c>
+      <c r="G112" s="1">
         <v>120</v>
       </c>
-      <c r="G112" s="1">
-        <v>0</v>
-      </c>
       <c r="H112" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I112" s="1">
         <v>0</v>
       </c>
       <c r="J112" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="K112" s="1">
         <v>30</v>
       </c>
       <c r="L112" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M112" s="1">
         <v>51</v>
@@ -5973,7 +5985,7 @@
         <v>26</v>
       </c>
       <c r="O112" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="113">
@@ -6005,13 +6017,13 @@
         <v>0</v>
       </c>
       <c r="J113" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="K113" s="1">
         <v>0</v>
       </c>
       <c r="L113" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M113" s="1">
         <v>52</v>
@@ -6020,7 +6032,7 @@
         <v>26</v>
       </c>
       <c r="O113" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114">
@@ -6037,28 +6049,28 @@
         <v>116</v>
       </c>
       <c r="E114" s="1">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="F114" s="1">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G114" s="1">
         <v>120</v>
       </c>
       <c r="H114" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I114" s="1">
         <v>12</v>
       </c>
       <c r="J114" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="K114" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L114" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M114" s="1">
         <v>53</v>
@@ -6067,7 +6079,7 @@
         <v>27</v>
       </c>
       <c r="O114" s="1">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115">
@@ -6099,13 +6111,13 @@
         <v>0</v>
       </c>
       <c r="J115" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="K115" s="1">
         <v>0</v>
       </c>
       <c r="L115" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M115" s="1">
         <v>54</v>
@@ -6114,7 +6126,7 @@
         <v>27</v>
       </c>
       <c r="O115" s="1">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116">
@@ -6131,28 +6143,28 @@
         <v>118</v>
       </c>
       <c r="E116" s="1">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="F116" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G116" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="H116" s="1">
+        <v>0</v>
+      </c>
+      <c r="I116" s="1">
         <v>12</v>
       </c>
-      <c r="I116" s="1">
-        <v>6</v>
-      </c>
       <c r="J116" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="K116" s="1">
         <v>15</v>
       </c>
       <c r="L116" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M116" s="1">
         <v>55</v>
@@ -6161,7 +6173,7 @@
         <v>28</v>
       </c>
       <c r="O116" s="1">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117">
@@ -6193,13 +6205,13 @@
         <v>0</v>
       </c>
       <c r="J117" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="K117" s="1">
         <v>0</v>
       </c>
       <c r="L117" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M117" s="1">
         <v>56</v>
@@ -6208,7 +6220,7 @@
         <v>28</v>
       </c>
       <c r="O117" s="1">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="118">
@@ -6225,28 +6237,28 @@
         <v>120</v>
       </c>
       <c r="E118" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F118" s="1">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G118" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H118" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I118" s="1">
         <v>0</v>
       </c>
       <c r="J118" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="K118" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="L118" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M118" s="1">
         <v>57</v>
@@ -6255,7 +6267,7 @@
         <v>29</v>
       </c>
       <c r="O118" s="1">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119">
@@ -6287,13 +6299,13 @@
         <v>0</v>
       </c>
       <c r="J119" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="K119" s="1">
         <v>0</v>
       </c>
       <c r="L119" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M119" s="1">
         <v>58</v>
@@ -6302,7 +6314,7 @@
         <v>29</v>
       </c>
       <c r="O119" s="1">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="120">
@@ -6322,25 +6334,25 @@
         <v>20</v>
       </c>
       <c r="F120" s="1">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G120" s="1">
         <v>80</v>
       </c>
       <c r="H120" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I120" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J120" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="K120" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="L120" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M120" s="1">
         <v>59</v>
@@ -6349,7 +6361,7 @@
         <v>30</v>
       </c>
       <c r="O120" s="1">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="121">
@@ -6381,13 +6393,13 @@
         <v>0</v>
       </c>
       <c r="J121" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="K121" s="1">
         <v>0</v>
       </c>
       <c r="L121" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M121" s="1">
         <v>60</v>
@@ -6396,7 +6408,7 @@
         <v>30</v>
       </c>
       <c r="O121" s="1">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>